<commit_message>
Updated test_1_procedure_and_notes.txt which documents change in understanding of data from test 1
</commit_message>
<xml_diff>
--- a/PID_Test_wAccel/Spreadsheet_data_1.xlsx
+++ b/PID_Test_wAccel/Spreadsheet_data_1.xlsx
@@ -5629,37 +5629,37 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="587"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>-0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>-0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>-0</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
+                  <c:v>-0</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>-0</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>-0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0</c:v>
+                  <c:v>-0</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>-0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0</c:v>
+                  <c:v>-0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0</c:v>
+                  <c:v>-0</c:v>
                 </c:pt>
                 <c:pt idx="11">
                   <c:v>0</c:v>
@@ -5668,10 +5668,10 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0</c:v>
+                  <c:v>-0</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0</c:v>
+                  <c:v>-0</c:v>
                 </c:pt>
                 <c:pt idx="15">
                   <c:v>0</c:v>
@@ -5680,7 +5680,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0</c:v>
+                  <c:v>-0</c:v>
                 </c:pt>
                 <c:pt idx="18">
                   <c:v>0.02</c:v>
@@ -5689,22 +5689,22 @@
                   <c:v>0.01</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>0</c:v>
+                  <c:v>-0</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>0</c:v>
+                  <c:v>-0</c:v>
                 </c:pt>
                 <c:pt idx="22">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>0</c:v>
+                  <c:v>-0</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>0</c:v>
+                  <c:v>-0</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>0</c:v>
+                  <c:v>-0</c:v>
                 </c:pt>
                 <c:pt idx="26">
                   <c:v>-0</c:v>
@@ -7318,7 +7318,7 @@
                   <c:v>-0</c:v>
                 </c:pt>
                 <c:pt idx="563">
-                  <c:v>0</c:v>
+                  <c:v>-0</c:v>
                 </c:pt>
                 <c:pt idx="564">
                   <c:v>-0.01</c:v>
@@ -10972,11 +10972,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="7365137"/>
-        <c:axId val="27194396"/>
+        <c:axId val="27929384"/>
+        <c:axId val="78142930"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="7365137"/>
+        <c:axId val="27929384"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11034,11 +11034,11 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="27194396"/>
+        <c:crossAx val="78142930"/>
         <c:crosses val="autoZero"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="27194396"/>
+        <c:axId val="78142930"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11096,7 +11096,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="7365137"/>
+        <c:crossAx val="27929384"/>
         <c:crosses val="autoZero"/>
       </c:valAx>
       <c:spPr>
@@ -11186,7 +11186,6 @@
               <a:solidFill>
                 <a:srgbClr val="004586"/>
               </a:solidFill>
-              <a:custDash/>
               <a:round/>
             </a:ln>
           </c:spPr>
@@ -14746,6 +14745,17 @@
         <c:ser>
           <c:idx val="1"/>
           <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$G$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Speed Controller 4</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
           <c:spPr>
             <a:solidFill>
               <a:srgbClr val="ff420e"/>
@@ -14754,7 +14764,6 @@
               <a:solidFill>
                 <a:srgbClr val="ff420e"/>
               </a:solidFill>
-              <a:custDash/>
               <a:round/>
             </a:ln>
           </c:spPr>
@@ -16539,6 +16548,1776 @@
               </c:numCache>
             </c:numRef>
           </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$G$2:$G$588</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="587"/>
+                <c:pt idx="0">
+                  <c:v>1384</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1384</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1437</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1437</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1380</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1380</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1342</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1342</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1332</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1332</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1402</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1402</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>2027</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>2027</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>1484</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>1484</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>1452</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>1452</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>1540</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>1540</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>2300</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>2300</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>2300</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>2300</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>2300</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>2300</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>2300</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>2300</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>2152</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>2152</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>2265</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>2265</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>2300</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>2300</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="100">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="101">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="102">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="103">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="104">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="105">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="106">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="107">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="108">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="109">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="110">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="111">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="112">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="113">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="114">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="115">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="116">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="117">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="118">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="119">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="120">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="121">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="122">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="123">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="124">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="125">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="126">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="127">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="128">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="129">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="130">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="131">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="132">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="133">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="134">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="135">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="136">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="137">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="138">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="139">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="140">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="141">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="142">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="143">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="144">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="145">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="146">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="147">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="148">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="149">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="150">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="151">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="152">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="153">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="154">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="155">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="156">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="157">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="158">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="159">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="160">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="161">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="162">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="163">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="164">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="165">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="166">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="167">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="168">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="169">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="170">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="171">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="172">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="173">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="174">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="175">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="176">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="177">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="178">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="179">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="180">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="181">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="182">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="183">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="184">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="185">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="186">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="187">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="188">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="189">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="190">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="191">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="192">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="193">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="194">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="195">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="196">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="197">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="198">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="199">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="200">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="201">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="202">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="203">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="204">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="205">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="206">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="207">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="208">
+                  <c:v>1480</c:v>
+                </c:pt>
+                <c:pt idx="209">
+                  <c:v>1480</c:v>
+                </c:pt>
+                <c:pt idx="210">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="211">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="212">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="213">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="214">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="215">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="216">
+                  <c:v>1536</c:v>
+                </c:pt>
+                <c:pt idx="217">
+                  <c:v>1536</c:v>
+                </c:pt>
+                <c:pt idx="218">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="219">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="220">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="221">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="222">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="223">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="224">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="225">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="226">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="227">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="228">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="229">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="230">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="231">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="232">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="233">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="234">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="235">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="236">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="237">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="238">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="239">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="240">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="241">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="242">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="243">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="244">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="245">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="246">
+                  <c:v>1577</c:v>
+                </c:pt>
+                <c:pt idx="247">
+                  <c:v>1577</c:v>
+                </c:pt>
+                <c:pt idx="248">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="249">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="250">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="251">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="252">
+                  <c:v>1382</c:v>
+                </c:pt>
+                <c:pt idx="253">
+                  <c:v>1382</c:v>
+                </c:pt>
+                <c:pt idx="254">
+                  <c:v>1452</c:v>
+                </c:pt>
+                <c:pt idx="255">
+                  <c:v>1452</c:v>
+                </c:pt>
+                <c:pt idx="256">
+                  <c:v>2142</c:v>
+                </c:pt>
+                <c:pt idx="257">
+                  <c:v>2142</c:v>
+                </c:pt>
+                <c:pt idx="258">
+                  <c:v>2283</c:v>
+                </c:pt>
+                <c:pt idx="259">
+                  <c:v>2283</c:v>
+                </c:pt>
+                <c:pt idx="260">
+                  <c:v>1626</c:v>
+                </c:pt>
+                <c:pt idx="261">
+                  <c:v>1626</c:v>
+                </c:pt>
+                <c:pt idx="262">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="263">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="264">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="265">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="266">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="267">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="268">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="269">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="270">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="271">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="272">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="273">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="274">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="275">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="276">
+                  <c:v>2300</c:v>
+                </c:pt>
+                <c:pt idx="277">
+                  <c:v>2300</c:v>
+                </c:pt>
+                <c:pt idx="278">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="279">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="280">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="281">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="282">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="283">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="284">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="285">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="286">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="287">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="288">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="289">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="290">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="291">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="292">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="293">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="294">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="295">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="296">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="297">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="298">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="299">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="300">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="301">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="302">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="303">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="304">
+                  <c:v>2147</c:v>
+                </c:pt>
+                <c:pt idx="305">
+                  <c:v>2147</c:v>
+                </c:pt>
+                <c:pt idx="306">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="307">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="308">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="309">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="310">
+                  <c:v>1532</c:v>
+                </c:pt>
+                <c:pt idx="311">
+                  <c:v>1532</c:v>
+                </c:pt>
+                <c:pt idx="312">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="313">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="314">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="315">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="316">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="317">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="318">
+                  <c:v>1335</c:v>
+                </c:pt>
+                <c:pt idx="319">
+                  <c:v>1335</c:v>
+                </c:pt>
+                <c:pt idx="320">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="321">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="322">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="323">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="324">
+                  <c:v>1462</c:v>
+                </c:pt>
+                <c:pt idx="325">
+                  <c:v>1462</c:v>
+                </c:pt>
+                <c:pt idx="326">
+                  <c:v>1567</c:v>
+                </c:pt>
+                <c:pt idx="327">
+                  <c:v>1567</c:v>
+                </c:pt>
+                <c:pt idx="328">
+                  <c:v>1307</c:v>
+                </c:pt>
+                <c:pt idx="329">
+                  <c:v>1307</c:v>
+                </c:pt>
+                <c:pt idx="330">
+                  <c:v>1632</c:v>
+                </c:pt>
+                <c:pt idx="331">
+                  <c:v>1632</c:v>
+                </c:pt>
+                <c:pt idx="332">
+                  <c:v>1364</c:v>
+                </c:pt>
+                <c:pt idx="333">
+                  <c:v>1364</c:v>
+                </c:pt>
+                <c:pt idx="334">
+                  <c:v>1514</c:v>
+                </c:pt>
+                <c:pt idx="335">
+                  <c:v>1514</c:v>
+                </c:pt>
+                <c:pt idx="336">
+                  <c:v>1367</c:v>
+                </c:pt>
+                <c:pt idx="337">
+                  <c:v>1367</c:v>
+                </c:pt>
+                <c:pt idx="338">
+                  <c:v>1743</c:v>
+                </c:pt>
+                <c:pt idx="339">
+                  <c:v>1743</c:v>
+                </c:pt>
+                <c:pt idx="340">
+                  <c:v>1513</c:v>
+                </c:pt>
+                <c:pt idx="341">
+                  <c:v>1513</c:v>
+                </c:pt>
+                <c:pt idx="342">
+                  <c:v>1416</c:v>
+                </c:pt>
+                <c:pt idx="343">
+                  <c:v>1416</c:v>
+                </c:pt>
+                <c:pt idx="344">
+                  <c:v>1679</c:v>
+                </c:pt>
+                <c:pt idx="345">
+                  <c:v>1679</c:v>
+                </c:pt>
+                <c:pt idx="346">
+                  <c:v>1423</c:v>
+                </c:pt>
+                <c:pt idx="347">
+                  <c:v>1423</c:v>
+                </c:pt>
+                <c:pt idx="348">
+                  <c:v>1780</c:v>
+                </c:pt>
+                <c:pt idx="349">
+                  <c:v>1780</c:v>
+                </c:pt>
+                <c:pt idx="350">
+                  <c:v>1321</c:v>
+                </c:pt>
+                <c:pt idx="351">
+                  <c:v>1321</c:v>
+                </c:pt>
+                <c:pt idx="352">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="353">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="354">
+                  <c:v>1570</c:v>
+                </c:pt>
+                <c:pt idx="355">
+                  <c:v>1570</c:v>
+                </c:pt>
+                <c:pt idx="356">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="357">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="358">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="359">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="360">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="361">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="362">
+                  <c:v>1435</c:v>
+                </c:pt>
+                <c:pt idx="363">
+                  <c:v>1435</c:v>
+                </c:pt>
+                <c:pt idx="364">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="365">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="366">
+                  <c:v>2119</c:v>
+                </c:pt>
+                <c:pt idx="367">
+                  <c:v>2119</c:v>
+                </c:pt>
+                <c:pt idx="368">
+                  <c:v>1525</c:v>
+                </c:pt>
+                <c:pt idx="369">
+                  <c:v>1525</c:v>
+                </c:pt>
+                <c:pt idx="370">
+                  <c:v>1567</c:v>
+                </c:pt>
+                <c:pt idx="371">
+                  <c:v>1567</c:v>
+                </c:pt>
+                <c:pt idx="372">
+                  <c:v>1504</c:v>
+                </c:pt>
+                <c:pt idx="373">
+                  <c:v>1504</c:v>
+                </c:pt>
+                <c:pt idx="374">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="375">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="376">
+                  <c:v>1623</c:v>
+                </c:pt>
+                <c:pt idx="377">
+                  <c:v>1623</c:v>
+                </c:pt>
+                <c:pt idx="378">
+                  <c:v>1451</c:v>
+                </c:pt>
+                <c:pt idx="379">
+                  <c:v>1451</c:v>
+                </c:pt>
+                <c:pt idx="380">
+                  <c:v>1321</c:v>
+                </c:pt>
+                <c:pt idx="381">
+                  <c:v>1321</c:v>
+                </c:pt>
+                <c:pt idx="382">
+                  <c:v>1598</c:v>
+                </c:pt>
+                <c:pt idx="383">
+                  <c:v>1598</c:v>
+                </c:pt>
+                <c:pt idx="384">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="385">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="386">
+                  <c:v>1560</c:v>
+                </c:pt>
+                <c:pt idx="387">
+                  <c:v>1560</c:v>
+                </c:pt>
+                <c:pt idx="388">
+                  <c:v>1611</c:v>
+                </c:pt>
+                <c:pt idx="389">
+                  <c:v>1611</c:v>
+                </c:pt>
+                <c:pt idx="390">
+                  <c:v>1406</c:v>
+                </c:pt>
+                <c:pt idx="391">
+                  <c:v>1406</c:v>
+                </c:pt>
+                <c:pt idx="392">
+                  <c:v>1480</c:v>
+                </c:pt>
+                <c:pt idx="393">
+                  <c:v>1480</c:v>
+                </c:pt>
+                <c:pt idx="394">
+                  <c:v>1407</c:v>
+                </c:pt>
+                <c:pt idx="395">
+                  <c:v>1407</c:v>
+                </c:pt>
+                <c:pt idx="396">
+                  <c:v>1433</c:v>
+                </c:pt>
+                <c:pt idx="397">
+                  <c:v>1433</c:v>
+                </c:pt>
+                <c:pt idx="398">
+                  <c:v>1656</c:v>
+                </c:pt>
+                <c:pt idx="399">
+                  <c:v>1656</c:v>
+                </c:pt>
+                <c:pt idx="400">
+                  <c:v>1623</c:v>
+                </c:pt>
+                <c:pt idx="401">
+                  <c:v>1623</c:v>
+                </c:pt>
+                <c:pt idx="402">
+                  <c:v>1388</c:v>
+                </c:pt>
+                <c:pt idx="403">
+                  <c:v>1388</c:v>
+                </c:pt>
+                <c:pt idx="404">
+                  <c:v>1679</c:v>
+                </c:pt>
+                <c:pt idx="405">
+                  <c:v>1679</c:v>
+                </c:pt>
+                <c:pt idx="406">
+                  <c:v>1379</c:v>
+                </c:pt>
+                <c:pt idx="407">
+                  <c:v>1379</c:v>
+                </c:pt>
+                <c:pt idx="408">
+                  <c:v>1612</c:v>
+                </c:pt>
+                <c:pt idx="409">
+                  <c:v>1612</c:v>
+                </c:pt>
+                <c:pt idx="410">
+                  <c:v>1641</c:v>
+                </c:pt>
+                <c:pt idx="411">
+                  <c:v>1641</c:v>
+                </c:pt>
+                <c:pt idx="412">
+                  <c:v>1514</c:v>
+                </c:pt>
+                <c:pt idx="413">
+                  <c:v>1514</c:v>
+                </c:pt>
+                <c:pt idx="414">
+                  <c:v>1680</c:v>
+                </c:pt>
+                <c:pt idx="415">
+                  <c:v>1680</c:v>
+                </c:pt>
+                <c:pt idx="416">
+                  <c:v>1595</c:v>
+                </c:pt>
+                <c:pt idx="417">
+                  <c:v>1595</c:v>
+                </c:pt>
+                <c:pt idx="418">
+                  <c:v>1418</c:v>
+                </c:pt>
+                <c:pt idx="419">
+                  <c:v>1418</c:v>
+                </c:pt>
+                <c:pt idx="420">
+                  <c:v>1828</c:v>
+                </c:pt>
+                <c:pt idx="421">
+                  <c:v>1828</c:v>
+                </c:pt>
+                <c:pt idx="422">
+                  <c:v>1501</c:v>
+                </c:pt>
+                <c:pt idx="423">
+                  <c:v>1501</c:v>
+                </c:pt>
+                <c:pt idx="424">
+                  <c:v>1359</c:v>
+                </c:pt>
+                <c:pt idx="425">
+                  <c:v>1359</c:v>
+                </c:pt>
+                <c:pt idx="426">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="427">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="428">
+                  <c:v>1504</c:v>
+                </c:pt>
+                <c:pt idx="429">
+                  <c:v>1504</c:v>
+                </c:pt>
+                <c:pt idx="430">
+                  <c:v>1430</c:v>
+                </c:pt>
+                <c:pt idx="431">
+                  <c:v>1430</c:v>
+                </c:pt>
+                <c:pt idx="432">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="433">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="434">
+                  <c:v>1417</c:v>
+                </c:pt>
+                <c:pt idx="435">
+                  <c:v>1417</c:v>
+                </c:pt>
+                <c:pt idx="436">
+                  <c:v>1778</c:v>
+                </c:pt>
+                <c:pt idx="437">
+                  <c:v>1778</c:v>
+                </c:pt>
+                <c:pt idx="438">
+                  <c:v>1734</c:v>
+                </c:pt>
+                <c:pt idx="439">
+                  <c:v>1734</c:v>
+                </c:pt>
+                <c:pt idx="440">
+                  <c:v>1697</c:v>
+                </c:pt>
+                <c:pt idx="441">
+                  <c:v>1697</c:v>
+                </c:pt>
+                <c:pt idx="442">
+                  <c:v>1818</c:v>
+                </c:pt>
+                <c:pt idx="443">
+                  <c:v>1818</c:v>
+                </c:pt>
+                <c:pt idx="444">
+                  <c:v>1446</c:v>
+                </c:pt>
+                <c:pt idx="445">
+                  <c:v>1446</c:v>
+                </c:pt>
+                <c:pt idx="446">
+                  <c:v>1638</c:v>
+                </c:pt>
+                <c:pt idx="447">
+                  <c:v>1638</c:v>
+                </c:pt>
+                <c:pt idx="448">
+                  <c:v>1950</c:v>
+                </c:pt>
+                <c:pt idx="449">
+                  <c:v>1950</c:v>
+                </c:pt>
+                <c:pt idx="450">
+                  <c:v>1579</c:v>
+                </c:pt>
+                <c:pt idx="451">
+                  <c:v>1579</c:v>
+                </c:pt>
+                <c:pt idx="452">
+                  <c:v>1542</c:v>
+                </c:pt>
+                <c:pt idx="453">
+                  <c:v>1542</c:v>
+                </c:pt>
+                <c:pt idx="454">
+                  <c:v>1807</c:v>
+                </c:pt>
+                <c:pt idx="455">
+                  <c:v>1807</c:v>
+                </c:pt>
+                <c:pt idx="456">
+                  <c:v>1725</c:v>
+                </c:pt>
+                <c:pt idx="457">
+                  <c:v>1725</c:v>
+                </c:pt>
+                <c:pt idx="458">
+                  <c:v>1717</c:v>
+                </c:pt>
+                <c:pt idx="459">
+                  <c:v>1717</c:v>
+                </c:pt>
+                <c:pt idx="460">
+                  <c:v>1586</c:v>
+                </c:pt>
+                <c:pt idx="461">
+                  <c:v>1586</c:v>
+                </c:pt>
+                <c:pt idx="462">
+                  <c:v>1715</c:v>
+                </c:pt>
+                <c:pt idx="463">
+                  <c:v>1715</c:v>
+                </c:pt>
+                <c:pt idx="464">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="465">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="466">
+                  <c:v>1431</c:v>
+                </c:pt>
+                <c:pt idx="467">
+                  <c:v>1431</c:v>
+                </c:pt>
+                <c:pt idx="468">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="469">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="470">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="471">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="472">
+                  <c:v>1312</c:v>
+                </c:pt>
+                <c:pt idx="473">
+                  <c:v>1312</c:v>
+                </c:pt>
+                <c:pt idx="474">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="475">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="476">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="477">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="478">
+                  <c:v>1374</c:v>
+                </c:pt>
+                <c:pt idx="479">
+                  <c:v>1374</c:v>
+                </c:pt>
+                <c:pt idx="480">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="481">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="482">
+                  <c:v>1820</c:v>
+                </c:pt>
+                <c:pt idx="483">
+                  <c:v>1820</c:v>
+                </c:pt>
+                <c:pt idx="484">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="485">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="486">
+                  <c:v>2082</c:v>
+                </c:pt>
+                <c:pt idx="487">
+                  <c:v>2082</c:v>
+                </c:pt>
+                <c:pt idx="488">
+                  <c:v>1586</c:v>
+                </c:pt>
+                <c:pt idx="489">
+                  <c:v>1586</c:v>
+                </c:pt>
+                <c:pt idx="490">
+                  <c:v>1673</c:v>
+                </c:pt>
+                <c:pt idx="491">
+                  <c:v>1673</c:v>
+                </c:pt>
+                <c:pt idx="492">
+                  <c:v>1532</c:v>
+                </c:pt>
+                <c:pt idx="493">
+                  <c:v>1532</c:v>
+                </c:pt>
+                <c:pt idx="494">
+                  <c:v>1517</c:v>
+                </c:pt>
+                <c:pt idx="495">
+                  <c:v>1517</c:v>
+                </c:pt>
+                <c:pt idx="496">
+                  <c:v>1819</c:v>
+                </c:pt>
+                <c:pt idx="497">
+                  <c:v>1819</c:v>
+                </c:pt>
+                <c:pt idx="498">
+                  <c:v>1602</c:v>
+                </c:pt>
+                <c:pt idx="499">
+                  <c:v>1602</c:v>
+                </c:pt>
+                <c:pt idx="500">
+                  <c:v>1457</c:v>
+                </c:pt>
+                <c:pt idx="501">
+                  <c:v>1457</c:v>
+                </c:pt>
+                <c:pt idx="502">
+                  <c:v>1635</c:v>
+                </c:pt>
+                <c:pt idx="503">
+                  <c:v>1635</c:v>
+                </c:pt>
+                <c:pt idx="504">
+                  <c:v>1627</c:v>
+                </c:pt>
+                <c:pt idx="505">
+                  <c:v>1627</c:v>
+                </c:pt>
+                <c:pt idx="506">
+                  <c:v>1623</c:v>
+                </c:pt>
+                <c:pt idx="507">
+                  <c:v>1623</c:v>
+                </c:pt>
+                <c:pt idx="508">
+                  <c:v>2300</c:v>
+                </c:pt>
+                <c:pt idx="509">
+                  <c:v>2300</c:v>
+                </c:pt>
+                <c:pt idx="510">
+                  <c:v>2300</c:v>
+                </c:pt>
+                <c:pt idx="511">
+                  <c:v>2300</c:v>
+                </c:pt>
+                <c:pt idx="512">
+                  <c:v>2300</c:v>
+                </c:pt>
+                <c:pt idx="513">
+                  <c:v>2300</c:v>
+                </c:pt>
+                <c:pt idx="514">
+                  <c:v>2300</c:v>
+                </c:pt>
+                <c:pt idx="515">
+                  <c:v>2300</c:v>
+                </c:pt>
+                <c:pt idx="516">
+                  <c:v>2300</c:v>
+                </c:pt>
+                <c:pt idx="517">
+                  <c:v>2300</c:v>
+                </c:pt>
+                <c:pt idx="518">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="519">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="520">
+                  <c:v>2300</c:v>
+                </c:pt>
+                <c:pt idx="521">
+                  <c:v>2300</c:v>
+                </c:pt>
+                <c:pt idx="522">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="523">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="524">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="525">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="526">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="527">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="528">
+                  <c:v>2300</c:v>
+                </c:pt>
+                <c:pt idx="529">
+                  <c:v>2300</c:v>
+                </c:pt>
+                <c:pt idx="530">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="531">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="532">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="533">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="534">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="535">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="536">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="537">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="538">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="539">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="540">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="541">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="542">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="543">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="544">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="545">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="546">
+                  <c:v>2300</c:v>
+                </c:pt>
+                <c:pt idx="547">
+                  <c:v>2300</c:v>
+                </c:pt>
+                <c:pt idx="548">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="549">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="550">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="551">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="552">
+                  <c:v>2300</c:v>
+                </c:pt>
+                <c:pt idx="553">
+                  <c:v>2300</c:v>
+                </c:pt>
+                <c:pt idx="554">
+                  <c:v>2300</c:v>
+                </c:pt>
+                <c:pt idx="555">
+                  <c:v>2300</c:v>
+                </c:pt>
+                <c:pt idx="556">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="557">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="558">
+                  <c:v>1720</c:v>
+                </c:pt>
+                <c:pt idx="559">
+                  <c:v>1720</c:v>
+                </c:pt>
+                <c:pt idx="560">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="561">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="562">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="563">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="564">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="565">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="566">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="567">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="568">
+                  <c:v>1354</c:v>
+                </c:pt>
+                <c:pt idx="569">
+                  <c:v>1354</c:v>
+                </c:pt>
+                <c:pt idx="570">
+                  <c:v>1361</c:v>
+                </c:pt>
+                <c:pt idx="571">
+                  <c:v>1361</c:v>
+                </c:pt>
+                <c:pt idx="572">
+                  <c:v>1377</c:v>
+                </c:pt>
+                <c:pt idx="573">
+                  <c:v>1377</c:v>
+                </c:pt>
+                <c:pt idx="574">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="575">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="576">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="577">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="578">
+                  <c:v>1518</c:v>
+                </c:pt>
+                <c:pt idx="579">
+                  <c:v>1518</c:v>
+                </c:pt>
+                <c:pt idx="580">
+                  <c:v>1406</c:v>
+                </c:pt>
+                <c:pt idx="581">
+                  <c:v>1406</c:v>
+                </c:pt>
+                <c:pt idx="582">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="583">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="584">
+                  <c:v>2211</c:v>
+                </c:pt>
+                <c:pt idx="585">
+                  <c:v>2211</c:v>
+                </c:pt>
+                <c:pt idx="586">
+                  <c:v>2300</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
         <c:ser>
@@ -20119,11 +21898,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="20942335"/>
-        <c:axId val="25242178"/>
+        <c:axId val="58939715"/>
+        <c:axId val="93429305"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="20942335"/>
+        <c:axId val="58939715"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -20172,11 +21951,11 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="25242178"/>
+        <c:crossAx val="93429305"/>
         <c:crosses val="autoZero"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="25242178"/>
+        <c:axId val="93429305"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -20234,7 +22013,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="20942335"/>
+        <c:crossAx val="58939715"/>
         <c:crosses val="autoZero"/>
       </c:valAx>
       <c:spPr>
@@ -20324,7 +22103,6 @@
               <a:solidFill>
                 <a:srgbClr val="3333ff"/>
               </a:solidFill>
-              <a:custDash/>
               <a:round/>
             </a:ln>
           </c:spPr>
@@ -23903,7 +25681,6 @@
               <a:solidFill>
                 <a:srgbClr val="ff0000"/>
               </a:solidFill>
-              <a:custDash/>
               <a:round/>
             </a:ln>
           </c:spPr>
@@ -25695,37 +27472,37 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="587"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>-0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>-0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>-0</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
+                  <c:v>-0</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>-0</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>-0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0</c:v>
+                  <c:v>-0</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>-0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0</c:v>
+                  <c:v>-0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0</c:v>
+                  <c:v>-0</c:v>
                 </c:pt>
                 <c:pt idx="11">
                   <c:v>0</c:v>
@@ -25734,10 +27511,10 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0</c:v>
+                  <c:v>-0</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0</c:v>
+                  <c:v>-0</c:v>
                 </c:pt>
                 <c:pt idx="15">
                   <c:v>0</c:v>
@@ -25746,7 +27523,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0</c:v>
+                  <c:v>-0</c:v>
                 </c:pt>
                 <c:pt idx="18">
                   <c:v>0.02</c:v>
@@ -25755,22 +27532,22 @@
                   <c:v>0.01</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>0</c:v>
+                  <c:v>-0</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>0</c:v>
+                  <c:v>-0</c:v>
                 </c:pt>
                 <c:pt idx="22">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>0</c:v>
+                  <c:v>-0</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>0</c:v>
+                  <c:v>-0</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>0</c:v>
+                  <c:v>-0</c:v>
                 </c:pt>
                 <c:pt idx="26">
                   <c:v>-0</c:v>
@@ -27384,7 +29161,7 @@
                   <c:v>-0</c:v>
                 </c:pt>
                 <c:pt idx="563">
-                  <c:v>0</c:v>
+                  <c:v>-0</c:v>
                 </c:pt>
                 <c:pt idx="564">
                   <c:v>-0.01</c:v>
@@ -27482,7 +29259,6 @@
               <a:solidFill>
                 <a:srgbClr val="66ff00"/>
               </a:solidFill>
-              <a:custDash/>
               <a:round/>
             </a:ln>
           </c:spPr>
@@ -31061,7 +32837,6 @@
               <a:solidFill>
                 <a:srgbClr val="7e0021"/>
               </a:solidFill>
-              <a:custDash/>
               <a:round/>
             </a:ln>
           </c:spPr>
@@ -34640,7 +36415,6 @@
               <a:solidFill>
                 <a:srgbClr val="6699cc"/>
               </a:solidFill>
-              <a:custDash/>
               <a:round/>
             </a:ln>
           </c:spPr>
@@ -38219,7 +39993,6 @@
               <a:solidFill>
                 <a:srgbClr val="669966"/>
               </a:solidFill>
-              <a:custDash/>
               <a:round/>
             </a:ln>
           </c:spPr>
@@ -41776,11 +43549,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="10872041"/>
-        <c:axId val="63008606"/>
+        <c:axId val="40799286"/>
+        <c:axId val="52783611"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="10872041"/>
+        <c:axId val="40799286"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -41829,11 +43602,11 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="63008606"/>
+        <c:crossAx val="52783611"/>
         <c:crosses val="autoZero"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="63008606"/>
+        <c:axId val="52783611"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -41891,7 +43664,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="10872041"/>
+        <c:crossAx val="40799286"/>
         <c:crosses val="autoZero"/>
       </c:valAx>
       <c:spPr>
@@ -42040,7 +43813,7 @@
   <dimension ref="A1:J588"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H1" activeCellId="0" sqref="H1"/>
+      <selection pane="topLeft" activeCell="J2" activeCellId="0" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -63220,11 +64993,11 @@
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+    <oddHeader>&amp;C&amp;A</oddHeader>
+    <oddFooter>&amp;CPage &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
@@ -63246,11 +65019,11 @@
   </cols>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+    <oddHeader>&amp;C&amp;A</oddHeader>
+    <oddFooter>&amp;CPage &amp;P</oddFooter>
   </headerFooter>
   <drawing r:id="rId1"/>
 </worksheet>
@@ -63273,11 +65046,11 @@
   </cols>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+    <oddHeader>&amp;C&amp;A</oddHeader>
+    <oddFooter>&amp;CPage &amp;P</oddFooter>
   </headerFooter>
   <drawing r:id="rId1"/>
 </worksheet>
@@ -63300,11 +65073,11 @@
   </cols>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+    <oddHeader>&amp;C&amp;A</oddHeader>
+    <oddFooter>&amp;CPage &amp;P</oddFooter>
   </headerFooter>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Updated analysis of data.  Most likely last analysis on current data set pending updated testing using Y-axis control.  Consideration of any response differences between different motor controllers is appropriate to better analyze the data of future tests.
</commit_message>
<xml_diff>
--- a/PID_Test_wAccel/Spreadsheet_data_1.xlsx
+++ b/PID_Test_wAccel/Spreadsheet_data_1.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -205,7 +205,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -259,7 +259,6 @@
               <a:solidFill>
                 <a:srgbClr val="004586"/>
               </a:solidFill>
-              <a:custDash/>
               <a:round/>
             </a:ln>
           </c:spPr>
@@ -10972,11 +10971,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="27929384"/>
-        <c:axId val="78142930"/>
+        <c:axId val="48230553"/>
+        <c:axId val="5591450"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="27929384"/>
+        <c:axId val="48230553"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11034,11 +11033,11 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="78142930"/>
+        <c:crossAx val="5591450"/>
         <c:crosses val="autoZero"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="78142930"/>
+        <c:axId val="5591450"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11096,7 +11095,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="27929384"/>
+        <c:crossAx val="48230553"/>
         <c:crosses val="autoZero"/>
       </c:valAx>
       <c:spPr>
@@ -11132,7 +11131,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -21898,11 +21897,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="58939715"/>
-        <c:axId val="93429305"/>
+        <c:axId val="88852478"/>
+        <c:axId val="75695807"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="58939715"/>
+        <c:axId val="88852478"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -21951,11 +21950,11 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="93429305"/>
+        <c:crossAx val="75695807"/>
         <c:crosses val="autoZero"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="93429305"/>
+        <c:axId val="75695807"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -22013,7 +22012,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="58939715"/>
+        <c:crossAx val="88852478"/>
         <c:crosses val="autoZero"/>
       </c:valAx>
       <c:spPr>
@@ -22049,7 +22048,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -43549,11 +43548,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="40799286"/>
-        <c:axId val="52783611"/>
+        <c:axId val="13675620"/>
+        <c:axId val="82132507"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="40799286"/>
+        <c:axId val="13675620"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -43602,11 +43601,11 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="52783611"/>
+        <c:crossAx val="82132507"/>
         <c:crosses val="autoZero"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="52783611"/>
+        <c:axId val="82132507"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -43664,7 +43663,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="40799286"/>
+        <c:crossAx val="13675620"/>
         <c:crosses val="autoZero"/>
       </c:valAx>
       <c:spPr>
@@ -65036,7 +65035,7 @@
   </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="R22" activeCellId="0" sqref="R22"/>
     </sheetView>
   </sheetViews>
@@ -65063,7 +65062,7 @@
   </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="P17" activeCellId="0" sqref="P17"/>
     </sheetView>
   </sheetViews>

</xml_diff>